<commit_message>
Added counts for Publication Language
</commit_message>
<xml_diff>
--- a/Excel Output/Duplicates.xlsx
+++ b/Excel Output/Duplicates.xlsx
@@ -29,7 +29,7 @@
     <t>10</t>
   </si>
   <si>
-    <t>242</t>
+    <t>238</t>
   </si>
   <si>
     <t>91</t>
@@ -47,136 +47,136 @@
     <t>11</t>
   </si>
   <si>
-    <t>243</t>
+    <t>239</t>
   </si>
   <si>
     <t>203</t>
   </si>
   <si>
+    <t>288</t>
+  </si>
+  <si>
+    <t>205</t>
+  </si>
+  <si>
+    <t>291</t>
+  </si>
+  <si>
+    <t>208</t>
+  </si>
+  <si>
     <t>292</t>
   </si>
   <si>
-    <t>205</t>
-  </si>
-  <si>
-    <t>295</t>
-  </si>
-  <si>
-    <t>208</t>
+    <t>134</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>209</t>
+  </si>
+  <si>
+    <t>273</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>157</t>
+  </si>
+  <si>
+    <t>158</t>
+  </si>
+  <si>
+    <t>159</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>162</t>
+  </si>
+  <si>
+    <t>163</t>
+  </si>
+  <si>
+    <t>164</t>
+  </si>
+  <si>
+    <t>165</t>
+  </si>
+  <si>
+    <t>166</t>
+  </si>
+  <si>
+    <t>167</t>
+  </si>
+  <si>
+    <t>168</t>
+  </si>
+  <si>
+    <t>169</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>171</t>
+  </si>
+  <si>
+    <t>172</t>
+  </si>
+  <si>
+    <t>173</t>
   </si>
   <si>
     <t>296</t>
   </si>
   <si>
-    <t>134</t>
-  </si>
-  <si>
-    <t>135</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>244</t>
-  </si>
-  <si>
-    <t>140</t>
-  </si>
-  <si>
-    <t>141</t>
-  </si>
-  <si>
-    <t>146</t>
-  </si>
-  <si>
-    <t>147</t>
-  </si>
-  <si>
-    <t>209</t>
-  </si>
-  <si>
-    <t>277</t>
-  </si>
-  <si>
-    <t>148</t>
-  </si>
-  <si>
-    <t>149</t>
-  </si>
-  <si>
-    <t>151</t>
-  </si>
-  <si>
-    <t>152</t>
-  </si>
-  <si>
-    <t>153</t>
-  </si>
-  <si>
-    <t>154</t>
-  </si>
-  <si>
-    <t>155</t>
-  </si>
-  <si>
-    <t>156</t>
-  </si>
-  <si>
-    <t>157</t>
-  </si>
-  <si>
-    <t>158</t>
-  </si>
-  <si>
-    <t>159</t>
-  </si>
-  <si>
-    <t>160</t>
-  </si>
-  <si>
-    <t>161</t>
-  </si>
-  <si>
-    <t>162</t>
-  </si>
-  <si>
-    <t>163</t>
-  </si>
-  <si>
-    <t>164</t>
-  </si>
-  <si>
-    <t>165</t>
-  </si>
-  <si>
-    <t>166</t>
-  </si>
-  <si>
-    <t>167</t>
-  </si>
-  <si>
-    <t>168</t>
-  </si>
-  <si>
-    <t>169</t>
-  </si>
-  <si>
-    <t>170</t>
-  </si>
-  <si>
-    <t>171</t>
-  </si>
-  <si>
-    <t>172</t>
-  </si>
-  <si>
-    <t>173</t>
-  </si>
-  <si>
-    <t>300</t>
-  </si>
-  <si>
-    <t>302</t>
+    <t>298</t>
   </si>
   <si>
     <t>184</t>
@@ -188,10 +188,10 @@
     <t>212</t>
   </si>
   <si>
-    <t>285</t>
-  </si>
-  <si>
-    <t>305</t>
+    <t>281</t>
+  </si>
+  <si>
+    <t>301</t>
   </si>
   <si>
     <t>28</t>
@@ -203,13 +203,13 @@
     <t>46</t>
   </si>
   <si>
-    <t>241</t>
+    <t>237</t>
   </si>
   <si>
     <t>9</t>
   </si>
   <si>
-    <t>269</t>
+    <t>265</t>
   </si>
   <si>
     <t>72</t>

</xml_diff>